<commit_message>
Updated App and Firmware
</commit_message>
<xml_diff>
--- a/Timesheets/2019-04-14.xlsx
+++ b/Timesheets/2019-04-14.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdemolde\Documents\GitHub\Coleman-Nordic-Butterfly\Timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818D4F6E-E92A-4E40-A2DB-36A4B41FFAF0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB43172-1214-4C8D-B9E3-B8C2A74C4A69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12645" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="timesheet.hourly" sheetId="1" r:id="rId1"/>
@@ -1620,7 +1620,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75"/>
@@ -1914,22 +1914,32 @@
       <c r="D12" s="37">
         <v>5.25</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="38">
+        <v>3.5</v>
+      </c>
       <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="G12" s="38">
+        <v>3.75</v>
+      </c>
+      <c r="H12" s="38">
+        <v>1.5</v>
+      </c>
       <c r="I12" s="38"/>
       <c r="J12" s="39"/>
       <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
+      <c r="L12" s="38">
+        <v>4.5</v>
+      </c>
       <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
+      <c r="N12" s="38">
+        <v>4.25</v>
+      </c>
       <c r="O12" s="38"/>
       <c r="P12" s="38"/>
       <c r="Q12" s="39"/>
       <c r="R12" s="55">
         <f t="shared" ref="R12:R21" si="0">SUM(D12:Q12)</f>
-        <v>5.25</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="33" customHeight="1" thickBot="1">
@@ -2159,7 +2169,7 @@
       </c>
       <c r="E22" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F22" s="60">
         <f t="shared" si="1"/>
@@ -2167,11 +2177,11 @@
       </c>
       <c r="G22" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="H22" s="69">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I22" s="69">
         <f t="shared" si="1"/>
@@ -2187,7 +2197,7 @@
       </c>
       <c r="L22" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="M22" s="60">
         <f t="shared" si="1"/>
@@ -2195,7 +2205,7 @@
       </c>
       <c r="N22" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="O22" s="69">
         <f t="shared" si="1"/>
@@ -2211,7 +2221,7 @@
       </c>
       <c r="R22" s="58">
         <f>SUM(D22:Q22)</f>
-        <v>5.25</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="29.1" customHeight="1">

</xml_diff>